<commit_message>
22.07.2018_Commit after including the PO related Scenarios
</commit_message>
<xml_diff>
--- a/Resources/Data/OrderType.xlsx
+++ b/Resources/Data/OrderType.xlsx
@@ -9,16 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7155" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20370" windowHeight="7155" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SDOrder" sheetId="1" r:id="rId1"/>
     <sheet name="MercentOrder" sheetId="3" r:id="rId2"/>
     <sheet name="DFSOrder" sheetId="4" r:id="rId3"/>
     <sheet name="Petnet" sheetId="11" r:id="rId4"/>
-    <sheet name="PALSReward" sheetId="5" r:id="rId5"/>
-    <sheet name="Petco_CC+GC" sheetId="6" r:id="rId6"/>
-    <sheet name="PO" sheetId="12" r:id="rId7"/>
+    <sheet name="PO" sheetId="12" r:id="rId5"/>
+    <sheet name="PALSReward" sheetId="5" r:id="rId6"/>
+    <sheet name="Petco_CC+GC" sheetId="6" r:id="rId7"/>
     <sheet name="BundledSKU" sheetId="8" r:id="rId8"/>
     <sheet name="GiftItem" sheetId="7" r:id="rId9"/>
     <sheet name="DonationItem" sheetId="9" r:id="rId10"/>
@@ -2845,8 +2845,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3004,6 +3004,81 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="232" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -3095,7 +3170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:A12"/>
@@ -3166,79 +3241,6 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:A11"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="232" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>